<commit_message>
Pruebas con Datos obtenidos fuera del tanque. Se agregó gitignore para evitar compartir archivos pesados (la data). Pendiente de datos en tanque todavía....
</commit_message>
<xml_diff>
--- a/Pruebas PMT.xlsx
+++ b/Pruebas PMT.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>V</t>
   </si>
@@ -52,6 +53,9 @@
   <si>
     <t>X</t>
   </si>
+  <si>
+    <t>x</t>
+  </si>
 </sst>
 </file>
 
@@ -66,7 +70,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -76,6 +80,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -107,11 +117,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -446,11 +457,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="228243120"/>
-        <c:axId val="228247040"/>
+        <c:axId val="240303096"/>
+        <c:axId val="240303880"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="228243120"/>
+        <c:axId val="240303096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -524,12 +535,12 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="228247040"/>
+        <c:crossAx val="240303880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="228247040"/>
+        <c:axId val="240303880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -631,7 +642,513 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="228243120"/>
+        <c:crossAx val="240303096"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-ES"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.31895909886264218"/>
+                  <c:y val="-1.8935185185185208E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="es-ES"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$A$3:$A$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1100</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1400</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$B$3:$B$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>116</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>183</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>251</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>319</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>387</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>456</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>525</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>592</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>662</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>730</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>798</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>867</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>937</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="242621744"/>
+        <c:axId val="242627624"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="242621744"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-ES"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="242627624"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="242627624"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-ES"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="242621744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -752,7 +1269,563 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1286,6 +2359,41 @@
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1568,8 +2676,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:Q27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="Q18" sqref="Q18"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1820,4 +2928,145 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:Q16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q17" sqref="Q17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>100</v>
+      </c>
+      <c r="B3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>200</v>
+      </c>
+      <c r="B4">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>300</v>
+      </c>
+      <c r="B5">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>400</v>
+      </c>
+      <c r="B6">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>500</v>
+      </c>
+      <c r="B7">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>600</v>
+      </c>
+      <c r="B8">
+        <v>387</v>
+      </c>
+      <c r="P8" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q8" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>700</v>
+      </c>
+      <c r="B9">
+        <v>456</v>
+      </c>
+      <c r="P9" s="2">
+        <f>Q9*0.6833 - 21.648</f>
+        <v>46.682000000000002</v>
+      </c>
+      <c r="Q9" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>800</v>
+      </c>
+      <c r="B10">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>900</v>
+      </c>
+      <c r="B11">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1000</v>
+      </c>
+      <c r="B12">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>1100</v>
+      </c>
+      <c r="B13">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>1200</v>
+      </c>
+      <c r="B14">
+        <v>798</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>1300</v>
+      </c>
+      <c r="B15">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>1400</v>
+      </c>
+      <c r="B16">
+        <v>937</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>